<commit_message>
Changed the compactToken parser for creating IRI tokens.
</commit_message>
<xml_diff>
--- a/Game.xlsx
+++ b/Game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurtc\Downloads\Code\semantical\ingestor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DE6AC4-E935-45E6-93D9-475403B0FBC9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E686C408-B69C-40F3-B4CD-755DB65AAD4F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7815" xr2:uid="{BC5F1D8A-A0E0-4BD1-A41E-4FE8D8900A7B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7815" activeTab="2" xr2:uid="{BC5F1D8A-A0E0-4BD1-A41E-4FE8D8900A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Term" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="255">
   <si>
     <t>Gender</t>
   </si>
@@ -222,6 +222,9 @@
     <t>Wyr</t>
   </si>
   <si>
+    <t>Vampyr</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -588,12 +591,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Aleria</t>
-  </si>
-  <si>
-    <t>An intelligenct young witch</t>
-  </si>
-  <si>
     <t>attribute</t>
   </si>
   <si>
@@ -706,6 +703,96 @@
   </si>
   <si>
     <t>The faceless minions of government (or any authority). They represent that authority in some manner, whether as tax collector, permit giver, or quiet enforcer. Powerful as both allies and enemies.</t>
+  </si>
+  <si>
+    <t>Grendak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A watch guard, not terribly bright, who Is just doing his job. He smells of onions and too many days unwashed, and normally looks slightly unshaven. </t>
+  </si>
+  <si>
+    <t>Apparent Age</t>
+  </si>
+  <si>
+    <t>The age an individual appears to be. This may differ wildly from their actual age, especially between species.</t>
+  </si>
+  <si>
+    <t>Young Child</t>
+  </si>
+  <si>
+    <t>The individual appears as a human child below the age of six.</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>The individual appears as a human child between six and ten.</t>
+  </si>
+  <si>
+    <t>The individual appears as a human child between ten and fourteen.</t>
+  </si>
+  <si>
+    <t>Teenager</t>
+  </si>
+  <si>
+    <t>The individual appears as a human child between fourteen and eighteen. Most teenagers have some legal rights, and are considered old enough to be consorted, though not yet married.</t>
+  </si>
+  <si>
+    <t>Young Adult</t>
+  </si>
+  <si>
+    <t>The individual appears to be between eighteen and twenty five. They are considered adults by society at this age.</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The individual appears to be between twenty five and thirty eight. This is considered physical prime. </t>
+  </si>
+  <si>
+    <t>Younger Middle Aged</t>
+  </si>
+  <si>
+    <t>Someone who appears between thirty eight and fifty. Hair is receding, body loses tone.</t>
+  </si>
+  <si>
+    <t>Older Middle Aged</t>
+  </si>
+  <si>
+    <t>Someone who appears to be aged between fifty and sixty five. Muscle has turned to fat, strength is diminishing, injuries are adding up.</t>
+  </si>
+  <si>
+    <t>Elderly</t>
+  </si>
+  <si>
+    <t>Someone between sixty five and eighty. Physical deterioration is accelerating, bones become weaker, hair has turned gray.</t>
+  </si>
+  <si>
+    <t>Ancient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Someone older than eighty. Bones are frail and systems are beginning to fail, hair has turned white, body has lost height. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A vampire is not an actual species, but rather is an undead version of other species controlled by a "demonic" parasite. Bodily decay is slowed by dark magic, and over time, physical limbs and organs are replaced by a magical simulcrum that can decorporealize. Elves and Dwarves are immune to vampyrization, but humans, fae, and magi are not. </t>
+  </si>
+  <si>
+    <t>Sevilla</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>An intelligent young witch</t>
+  </si>
+  <si>
+    <t>An urban fairy, normally appearing like a ragamuffin, quick with her fingers. She normally dresses like a boy and uses a subtle glamour. She has a fair amount of magic, but most of it gets channeled into finding shinies and punishing nobs who abuse street children.</t>
+  </si>
+  <si>
+    <t>Mara GlynisDottir</t>
   </si>
 </sst>
 </file>
@@ -1104,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4040E8-39A4-4EE4-B4EA-F3BD336EA04B}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E31" sqref="A31:XFD31"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,10 +1216,10 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1254,18 +1341,18 @@
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -1276,7 +1363,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="195" x14ac:dyDescent="0.25">
@@ -1287,34 +1374,34 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
@@ -1325,29 +1412,29 @@
     </row>
     <row r="18" spans="1:4" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -1356,20 +1443,20 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>15</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1378,9 +1465,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1389,9 +1476,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -1400,9 +1487,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
@@ -1413,7 +1500,7 @@
     </row>
     <row r="26" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
@@ -1422,293 +1509,290 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>218</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>219</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="2" t="s">
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" s="2" t="s">
+    </row>
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E43">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E44">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>82</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>87</v>
+      <c r="C46" t="s">
+        <v>84</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" s="3">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>30</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>34</v>
+      <c r="A49" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>100</v>
@@ -1716,83 +1800,83 @@
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>106</v>
@@ -1800,83 +1884,83 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>46</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>184</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>114</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="B57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D57" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C57" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C58" t="s">
-        <v>120</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" t="s">
         <v>121</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C59" t="s">
-        <v>122</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" t="s">
         <v>126</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C61" t="s">
-        <v>127</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>130</v>
@@ -1884,114 +1968,238 @@
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" t="s">
+        <v>128</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C62" t="s">
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>132</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="B63" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="D63" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C63" t="s">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>135</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="B64" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="D64" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C64" t="s">
-        <v>138</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>138</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" t="s">
+        <v>139</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C65" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>141</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C67" t="s">
+        <v>145</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C67" t="s">
-        <v>147</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C68" t="s">
+        <v>148</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C68" t="s">
+    </row>
+    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>150</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="B69" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C69" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="D69" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" t="s">
         <v>213</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D70" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>215</v>
+    </row>
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>229</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>231</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>241</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>243</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>245</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>247</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2001,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B53409A-22C3-45F0-967D-550026451B10}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2013,17 +2221,18 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="19" max="23" width="9.140625" style="1"/>
-    <col min="24" max="24" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="20" max="25" width="9.140625" style="1"/>
+    <col min="26" max="26" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2034,70 +2243,76 @@
       <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="X1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>254</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -2106,67 +2321,230 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>9</v>
-      </c>
-      <c r="G2">
-        <v>12</v>
       </c>
       <c r="H2">
         <v>10</v>
       </c>
       <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
         <v>14</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>15</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>17</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>15</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>18</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>17</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>15</v>
       </c>
-      <c r="Q2">
-        <v>13</v>
-      </c>
       <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2">
         <v>14</v>
-      </c>
-      <c r="S2" s="1">
-        <v>35</v>
       </c>
       <c r="T2" s="1">
         <v>15</v>
       </c>
       <c r="U2" s="1">
+        <v>35</v>
+      </c>
+      <c r="V2" s="1">
+        <v>15</v>
+      </c>
+      <c r="W2" s="1">
         <v>12</v>
       </c>
-      <c r="V2" s="1">
+      <c r="X2" s="1">
         <v>135</v>
       </c>
-      <c r="W2" s="1">
+      <c r="Y2" s="1">
         <v>22</v>
       </c>
-      <c r="X2" t="s">
-        <v>187</v>
+      <c r="Z2" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>9</v>
+      </c>
+      <c r="O3">
+        <v>12</v>
+      </c>
+      <c r="P3">
+        <v>9</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>9</v>
+      </c>
+      <c r="S3">
+        <v>8</v>
+      </c>
+      <c r="T3" s="1">
+        <v>6</v>
+      </c>
+      <c r="U3" s="1">
+        <v>18</v>
+      </c>
+      <c r="V3" s="1">
+        <v>24</v>
+      </c>
+      <c r="W3" s="1">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>13</v>
+      </c>
+      <c r="M4">
+        <v>14</v>
+      </c>
+      <c r="N4">
+        <v>16</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>7</v>
+      </c>
+      <c r="Q4">
+        <v>16</v>
+      </c>
+      <c r="R4">
+        <v>13</v>
+      </c>
+      <c r="S4">
+        <v>15</v>
+      </c>
+      <c r="T4" s="1">
+        <v>16</v>
+      </c>
+      <c r="U4" s="1">
+        <v>24</v>
+      </c>
+      <c r="V4" s="1">
+        <v>19</v>
+      </c>
+      <c r="W4" s="1">
+        <v>15</v>
+      </c>
+      <c r="X4" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2178,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050162D5-ABB5-4269-A172-80F5664D399F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,145 +2569,145 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2345,10 +2723,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CEDD19-856F-4305-B132-E1E1775B5FAB}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,7 +2740,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2370,7 +2748,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2378,7 +2756,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2386,7 +2764,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2394,7 +2772,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -2402,15 +2780,23 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>